<commit_message>
Changes in OD status and catalogs
</commit_message>
<xml_diff>
--- a/src/assets/documents/FORMATO_LOTES_OD.xlsx
+++ b/src/assets/documents/FORMATO_LOTES_OD.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aemo/Documents/Bellarti/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aemo/Projects/bellarti-app/src/assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BB64834-AE0E-E641-BCFC-44E92CB38B2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB98C42-77FA-AF49-A492-979618A6DD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-33680" yWindow="8220" windowWidth="29400" windowHeight="18380" xr2:uid="{1D5BD34A-BB4D-1D40-A5A6-40123166A6AD}"/>
+    <workbookView xWindow="-25580" yWindow="500" windowWidth="25140" windowHeight="26600" activeTab="1" xr2:uid="{1D5BD34A-BB4D-1D40-A5A6-40123166A6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTES" sheetId="1" r:id="rId1"/>
     <sheet name="DATA" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,6 +28,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>LOTE</t>
   </si>
@@ -58,20 +60,83 @@
     <t>ESTATUS</t>
   </si>
   <si>
-    <t>PENDIENTE</t>
-  </si>
-  <si>
-    <t>EN PROGRESO</t>
-  </si>
-  <si>
-    <t>FINALIZADO</t>
+    <t>ÁREA</t>
+  </si>
+  <si>
+    <t>PORCENTAJE</t>
+  </si>
+  <si>
+    <t>COCINA</t>
+  </si>
+  <si>
+    <t>CLOSET</t>
+  </si>
+  <si>
+    <t>PUERTAS</t>
+  </si>
+  <si>
+    <t>M. DE B.</t>
+  </si>
+  <si>
+    <t>WALDRAS</t>
+  </si>
+  <si>
+    <t>INSTALACIÓN</t>
+  </si>
+  <si>
+    <t>Material Listo</t>
+  </si>
+  <si>
+    <t>Corte Blanco</t>
+  </si>
+  <si>
+    <t>Corte Color</t>
+  </si>
+  <si>
+    <t>Enchape</t>
+  </si>
+  <si>
+    <t>Armado</t>
+  </si>
+  <si>
+    <t>Embarque</t>
+  </si>
+  <si>
+    <t>Entintado</t>
+  </si>
+  <si>
+    <t>Cocina</t>
+  </si>
+  <si>
+    <t>Granito</t>
+  </si>
+  <si>
+    <t>Corte</t>
+  </si>
+  <si>
+    <t>Closets</t>
+  </si>
+  <si>
+    <t>Vestidor</t>
+  </si>
+  <si>
+    <t>Mueble de Baño</t>
+  </si>
+  <si>
+    <t>Puertas Int</t>
+  </si>
+  <si>
+    <t>Waldras</t>
+  </si>
+  <si>
+    <t>Vobo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +147,14 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -117,11 +190,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -436,10 +510,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14B2720-D5F0-4745-9848-15750F9D2DAC}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -448,9 +522,10 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -464,14 +539,20 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D551B0DA-023B-974E-BF7B-140EB9A4703F}">
           <x14:formula1>
             <xm:f>DATA!$A$2:$A$3</xm:f>
@@ -482,7 +563,19 @@
           <x14:formula1>
             <xm:f>DATA!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E1048576</xm:sqref>
+          <xm:sqref>E887:E1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EEF66A23-A1E9-0F43-8742-2C16B1FC0B33}">
+          <x14:formula1>
+            <xm:f>DATA!$B$2:$B$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>E2:E6 E8:E886</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D20CA3DA-C254-F847-814C-729209900360}">
+          <x14:formula1>
+            <xm:f>DATA!$C$2:$C$17</xm:f>
+          </x14:formula1>
+          <xm:sqref>F2:F1205</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -492,47 +585,136 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBFC4D2-1602-FD40-B954-3AD0AFF51ABF}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>10</v>
+      </c>
+      <c r="C3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>9</v>
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updates of: OD, Purchase order and materials
</commit_message>
<xml_diff>
--- a/src/assets/documents/FORMATO_LOTES_OD.xlsx
+++ b/src/assets/documents/FORMATO_LOTES_OD.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aemo/Projects/bellarti-app/src/assets/documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB98C42-77FA-AF49-A492-979618A6DD27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C682BD0B-1A09-FC46-A75F-44B707F2CFD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25580" yWindow="500" windowWidth="25140" windowHeight="26600" activeTab="1" xr2:uid="{1D5BD34A-BB4D-1D40-A5A6-40123166A6AD}"/>
+    <workbookView xWindow="-25580" yWindow="500" windowWidth="25140" windowHeight="26600" xr2:uid="{1D5BD34A-BB4D-1D40-A5A6-40123166A6AD}"/>
   </bookViews>
   <sheets>
     <sheet name="LOTES" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
   <si>
     <t>LOTE</t>
   </si>
@@ -55,81 +55,6 @@
   </si>
   <si>
     <t>MANZANA</t>
-  </si>
-  <si>
-    <t>ESTATUS</t>
-  </si>
-  <si>
-    <t>ÁREA</t>
-  </si>
-  <si>
-    <t>PORCENTAJE</t>
-  </si>
-  <si>
-    <t>COCINA</t>
-  </si>
-  <si>
-    <t>CLOSET</t>
-  </si>
-  <si>
-    <t>PUERTAS</t>
-  </si>
-  <si>
-    <t>M. DE B.</t>
-  </si>
-  <si>
-    <t>WALDRAS</t>
-  </si>
-  <si>
-    <t>INSTALACIÓN</t>
-  </si>
-  <si>
-    <t>Material Listo</t>
-  </si>
-  <si>
-    <t>Corte Blanco</t>
-  </si>
-  <si>
-    <t>Corte Color</t>
-  </si>
-  <si>
-    <t>Enchape</t>
-  </si>
-  <si>
-    <t>Armado</t>
-  </si>
-  <si>
-    <t>Embarque</t>
-  </si>
-  <si>
-    <t>Entintado</t>
-  </si>
-  <si>
-    <t>Cocina</t>
-  </si>
-  <si>
-    <t>Granito</t>
-  </si>
-  <si>
-    <t>Corte</t>
-  </si>
-  <si>
-    <t>Closets</t>
-  </si>
-  <si>
-    <t>Vestidor</t>
-  </si>
-  <si>
-    <t>Mueble de Baño</t>
-  </si>
-  <si>
-    <t>Puertas Int</t>
-  </si>
-  <si>
-    <t>Waldras</t>
-  </si>
-  <si>
-    <t>Vobo</t>
   </si>
 </sst>
 </file>
@@ -510,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14B2720-D5F0-4745-9848-15750F9D2DAC}">
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -522,10 +447,9 @@
     <col min="2" max="2" width="14" customWidth="1"/>
     <col min="3" max="3" width="15.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>5</v>
       </c>
@@ -537,45 +461,18 @@
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D551B0DA-023B-974E-BF7B-140EB9A4703F}">
           <x14:formula1>
             <xm:f>DATA!$A$2:$A$3</xm:f>
           </x14:formula1>
           <xm:sqref>C2:C232</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{E3F36DEB-8C0B-824E-8583-1840429696A0}">
-          <x14:formula1>
-            <xm:f>DATA!$B$2:$B$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>E887:E1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{EEF66A23-A1E9-0F43-8742-2C16B1FC0B33}">
-          <x14:formula1>
-            <xm:f>DATA!$B$2:$B$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>E2:E6 E8:E886</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D20CA3DA-C254-F847-814C-729209900360}">
-          <x14:formula1>
-            <xm:f>DATA!$C$2:$C$17</xm:f>
-          </x14:formula1>
-          <xm:sqref>F2:F1205</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -585,132 +482,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BBFC4D2-1602-FD40-B954-3AD0AFF51ABF}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:A3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:B1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>15</v>
-      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C14" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C15" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>